<commit_message>
Update price for Gamgol buffe
</commit_message>
<xml_diff>
--- a/weatherIDs.xlsx
+++ b/weatherIDs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9320" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -344,22 +344,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -370,6 +358,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -651,25 +651,27 @@
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="53" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="4"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -789,13 +791,13 @@
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -905,13 +907,13 @@
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="8"/>
+      <c r="D28" s="9"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
@@ -1018,7 +1020,7 @@
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="11">
+      <c r="A39" s="7">
         <v>531</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -1028,19 +1030,19 @@
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="10"/>
+      <c r="A40" s="6"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="8"/>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
@@ -1127,7 +1129,7 @@
       <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="11">
+      <c r="A51" s="7">
         <v>620</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -1137,7 +1139,7 @@
       <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="11">
+      <c r="A52" s="7">
         <v>621</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -1147,7 +1149,7 @@
       <c r="D52" s="1"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="11">
+      <c r="A53" s="7">
         <v>622</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -1157,22 +1159,22 @@
       <c r="D53" s="1"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="9"/>
+      <c r="A54" s="5"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="9"/>
+      <c r="A55" s="5"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D56" s="8"/>
+      <c r="D56" s="9"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
@@ -1292,13 +1294,13 @@
       <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B70" s="6">
+      <c r="B70" s="4">
         <v>800</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C70" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D70" s="8"/>
+      <c r="D70" s="9"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
@@ -1328,13 +1330,13 @@
       <c r="A75" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="B75" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C75" s="7" t="s">
+      <c r="C75" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D75" s="8"/>
+      <c r="D75" s="9"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">

</xml_diff>